<commit_message>
Update xlsx files & csv files
Update xlsx files & csv files
</commit_message>
<xml_diff>
--- a/Documents/Files/Map.xlsx
+++ b/Documents/Files/Map.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sparta_Coding_Club\TeamProject\TextRPG_TeamProject2nd\TextRPG_TeamProject2nd\Documents\Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F28C93A-BBF3-4832-953D-92F50A4F1257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28695" yWindow="-90" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="시트1" sheetId="1" r:id="rId4"/>
+    <sheet name="시트1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -34,33 +43,296 @@
     <t>DESC</t>
   </si>
   <si>
+    <t>0|10</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>마을 옆에 있는 작은 숲. 조그마한 몬스터들이 부대끼며 살아간다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작은 숲</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0|1|10</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2|11</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>우거진 숲지</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작은 숲에서 조금 더 들어가면 울창한 숲이 펼쳐진다. 조금은 워험하다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>가도 경계</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>숲과가도의 경계선. 거대 늑대가 출몰하는 구역.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10|11|12</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>13|14</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3|12</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>0|1|2|3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>4|5</t>
-  </si>
-  <si>
-    <t>작은숲</t>
-  </si>
-  <si>
-    <t>작은 몬스터들이 살아요.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>슬라임 늪지</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1|2|3|4|5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>슬라임 왕경</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>15|16</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>늑대 소굴</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>늑대</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>평야</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4|5|6|13|14|15|16</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>달빛 아래 고원</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>11|12|13|14</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>늑대들의 보금자리 소탕작전. 조사원의 말로는 안쪽에서 무는 용도인지 모를 제단이 발견되었다고 한다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>늑대들의 성지. 밤이 되면 위대한 존재의 하인이 강림한다. 신정한 사도가 내려오지 않길 바래야 할 것이다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>늑대들의 주신, 암월랑의 출몰지역. 별밤의 황홀함에 현혹되지 말어라. 그건 네 앞에 있다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>슬라임들이 살아가는 늪지. 다만, 늪은 없다. 예전에는 있었다고 한다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>슬라임</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>엠퍼러가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>산다는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전설의 연못. 도끼를 빠트리면 은도끼와 금도끼를 얻을 수 있다는 소문이 있었다.</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,39 +340,69 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -290,27 +592,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="22.63"/>
-    <col customWidth="1" min="7" max="7" width="25.63"/>
+    <col min="1" max="3" width="12.5703125" style="2"/>
+    <col min="4" max="4" width="22.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="2"/>
+    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="92.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -333,33 +641,193 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2">
+        <v>6</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="12.75">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="C7" s="2">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="1"/>
     </row>
-    <row r="7">
-      <c r="H7" s="2"/>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2">
+        <v>17</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>